<commit_message>
Improve and document logic of function parseRoundsTokensForPlayers
</commit_message>
<xml_diff>
--- a/docs/design/ScoreCalculation.xlsx
+++ b/docs/design/ScoreCalculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sportit/Data/Projects/Interview/Argenti/source/poker-challenge-ts-main/docs/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A22D230-6CA3-834D-9095-2FB2D4026CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA31397E-021D-1941-B23A-94D587AAB38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14260" yWindow="4980" windowWidth="28040" windowHeight="17440" xr2:uid="{385D55CB-FC49-E140-AD0C-9C78E1D37DEF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>FourOfAKind</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>FACTOR</t>
+  </si>
+  <si>
+    <t>High card</t>
   </si>
 </sst>
 </file>
@@ -163,12 +166,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -181,9 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E9121C-FD99-0A49-A2BE-C0E96B5911DE}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,12 +514,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="5">
+      <c r="B1" s="8">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="1">
         <v>0</v>
       </c>
@@ -572,15 +576,15 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="6">
+      <c r="B5" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="6">
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="9">
         <v>0</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -628,14 +632,14 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="5">
-        <v>2</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5">
+      <c r="B9" s="8">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8">
         <v>1</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="1">
         <v>0</v>
       </c>
@@ -686,17 +690,17 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="5">
-        <v>3</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="9">
-        <v>2</v>
-      </c>
-      <c r="E13" s="10">
+      <c r="B13" s="8">
+        <v>3</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6">
         <v>1</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="7">
         <v>0</v>
       </c>
     </row>
@@ -743,6 +747,68 @@
       <c r="G15">
         <f>B15*POWER($J$1, $B$13) + D15 *POWER($J$1,$D$13)+ E15 *POWER($J$1,$E$13)+F15 *POWER($J$1,$F$13)</f>
         <v>10640</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="12">
+        <v>5</v>
+      </c>
+      <c r="C17" s="12">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <f>B18*POWER($J$1, $B$17) + C18*POWER($J$1, $C$17) + D18 *POWER($J$1,$D$17)+ E18 *POWER($J$1,$E$17)+F18 *POWER($J$1,$F$17)</f>
+        <v>10733240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <f>B19*POWER($J$1, $B$17) + C19*POWER($J$1, $C$17) + D19 *POWER($J$1,$D$17)+ E19 *POWER($J$1,$E$17)+F19 *POWER($J$1,$F$17)</f>
+        <v>10482008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>